<commit_message>
« l'entourage » → « entourage »
</commit_message>
<xml_diff>
--- a/vaccins.xlsx
+++ b/vaccins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a650138\src\recovax\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BC1129-EC68-49A0-8232-8D13C67EC838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D494226E-EFB2-43FD-A0F7-1B8D08BE2022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -244,9 +244,6 @@
     <t>les personnes obèses avec un IMC égal ou supérieur à 40 kg/m2</t>
   </si>
   <si>
-    <t>l’entourage familial des nourrissons âgés de moins de 6 mois avec des facteurs de risque de grippe grave</t>
-  </si>
-  <si>
     <t>les personnes séjournant dans un établissement médico-social d’hébergement, quel que soit leur âge</t>
   </si>
   <si>
@@ -254,6 +251,9 @@
   </si>
   <si>
     <t>rattrapage ; femme</t>
+  </si>
+  <si>
+    <t>entourage familial des nourrissons âgés de moins de 6 mois avec des facteurs de risque de grippe grave</t>
   </si>
 </sst>
 </file>
@@ -292,6 +292,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -329,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -339,6 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,6 +371,14 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
@@ -812,6 +822,168 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>52</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>61</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2052" name="Button 4" descr="OK" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2052"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:noFill/>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-150" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Aptos Narrow"/>
+                </a:rPr>
+                <a:t>OK</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>52</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>61</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2051" name="Button 3" descr="Cancel" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2051"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:noFill/>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-150" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Aptos Narrow"/>
+                </a:rPr>
+                <a:t>Cancel</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -1034,15 +1206,15 @@
   <sheetData/>
   <sheetProtection sheet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2050" r:id="rId3" name="Button 2">
+            <control shapeId="2050" r:id="rId4" name="Button 2">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
@@ -1064,7 +1236,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2049" r:id="rId4" name="Button 3">
+            <control shapeId="2049" r:id="rId5" name="Button 3">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
@@ -1086,7 +1258,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1001" r:id="rId5" name="Button 2">
+            <control shapeId="2052" r:id="rId6" name="Button 4">
               <controlPr defaultSize="0" autoFill="0" autoPict="0" altText="OK">
                 <anchor moveWithCells="1">
                   <from>
@@ -1108,7 +1280,51 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1002" r:id="rId6" name="Button 3">
+            <control shapeId="2051" r:id="rId7" name="Button 3">
+              <controlPr defaultSize="0" autoFill="0" autoPict="0" altText="Cancel">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>52</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>61</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>66675</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1001" r:id="rId8" name="Button -23">
+              <controlPr defaultSize="0" autoFill="0" autoPict="0" altText="OK">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>52</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>61</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>66675</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1002" r:id="rId9" name="Button -22">
               <controlPr defaultSize="0" autoFill="0" autoPict="0" altText="Cancel">
                 <anchor moveWithCells="1">
                   <from>
@@ -1138,8 +1354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,10 +1512,10 @@
         <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1693,8 +1909,8 @@
       <c r="B41" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>65</v>
+      <c r="C41" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>17</v>
@@ -1708,7 +1924,7 @@
         <v>38</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>17</v>

</xml_diff>